<commit_message>
add time last update
</commit_message>
<xml_diff>
--- a/components/exhauster_backend/prepare/Маппинг сигналов.xlsx
+++ b/components/exhauster_backend/prepare/Маппинг сигналов.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alextolmy/www/app/2023_evraz_hackaton/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alextolmy/www/app/2023_evraz_hackaton/components/exhauster_backend/prepare/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE420500-BD73-8849-9C8F-F57A8BD61C8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E368BA6-5A36-5640-92C3-2D0F02BF8514}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20360" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Эксгаустер № 1 (У-171)" sheetId="4" r:id="rId1"/>
@@ -5254,8 +5254,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M122"/>
   <sheetViews>
-    <sheetView topLeftCell="A100" zoomScale="113" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D122" sqref="A1:D122"/>
+    <sheetView tabSelected="1" topLeftCell="A87" zoomScale="113" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D101" sqref="D101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -19631,7 +19631,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:H122"/>
   <sheetViews>
-    <sheetView topLeftCell="A87" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A93" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="D122" sqref="A1:D122"/>
     </sheetView>
   </sheetViews>
@@ -22767,8 +22767,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:H122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A87" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D122" sqref="A1:D122"/>
+    <sheetView topLeftCell="A96" zoomScale="138" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>